<commit_message>
added function to add number of days
</commit_message>
<xml_diff>
--- a/test_highlight.xlsx
+++ b/test_highlight.xlsx
@@ -91,7 +91,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -114,11 +114,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -232,7 +227,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -279,15 +274,11 @@
       <protection locked="1" hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="1" hidden="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="1" hidden="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2456,12 +2447,12 @@
       <c r="AC22" s="2" t="n"/>
       <c r="AD22" s="2" t="n"/>
       <c r="AE22" s="2" t="n"/>
-      <c r="AF22" s="19" t="inlineStr">
+      <c r="AF22" s="17" t="inlineStr">
         <is>
           <t>08:48</t>
         </is>
       </c>
-      <c r="AG22" s="19" t="n"/>
+      <c r="AG22" s="2" t="n"/>
       <c r="AH22" s="2" t="n"/>
       <c r="AI22" s="2" t="n"/>
       <c r="AJ22" s="2" t="n"/>
@@ -2497,7 +2488,7 @@
       <c r="BN22" s="2" t="n"/>
       <c r="BO22" s="2" t="n"/>
       <c r="BQ22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BR22" s="14">
         <f>IF(BQ22&gt;0,BQ22*$BR$8,"")</f>
@@ -2568,12 +2559,12 @@
       <c r="AC23" s="2" t="n"/>
       <c r="AD23" s="2" t="n"/>
       <c r="AE23" s="2" t="n"/>
-      <c r="AF23" s="19" t="inlineStr">
+      <c r="AF23" s="17" t="inlineStr">
         <is>
           <t>17:01</t>
         </is>
       </c>
-      <c r="AG23" s="19" t="n"/>
+      <c r="AG23" s="2" t="n"/>
       <c r="AH23" s="2" t="n"/>
       <c r="AI23" s="2" t="n"/>
       <c r="AJ23" s="2" t="n"/>
@@ -2929,18 +2920,18 @@
         </is>
       </c>
       <c r="AC26" s="2" t="n"/>
-      <c r="AD26" s="19" t="inlineStr">
+      <c r="AD26" s="17" t="inlineStr">
         <is>
           <t>09:11</t>
         </is>
       </c>
-      <c r="AE26" s="19" t="n"/>
-      <c r="AF26" s="19" t="inlineStr">
+      <c r="AE26" s="2" t="n"/>
+      <c r="AF26" s="17" t="inlineStr">
         <is>
           <t>09:17</t>
         </is>
       </c>
-      <c r="AG26" s="19" t="n"/>
+      <c r="AG26" s="2" t="n"/>
       <c r="AH26" s="2" t="n"/>
       <c r="AI26" s="2" t="n"/>
       <c r="AJ26" s="2" t="n"/>
@@ -3045,18 +3036,18 @@
         </is>
       </c>
       <c r="AC27" s="2" t="n"/>
-      <c r="AD27" s="19" t="inlineStr">
+      <c r="AD27" s="17" t="inlineStr">
         <is>
           <t>16:18</t>
         </is>
       </c>
-      <c r="AE27" s="19" t="n"/>
-      <c r="AF27" s="19" t="inlineStr">
+      <c r="AE27" s="2" t="n"/>
+      <c r="AF27" s="17" t="inlineStr">
         <is>
           <t>16:56</t>
         </is>
       </c>
-      <c r="AG27" s="19" t="n"/>
+      <c r="AG27" s="2" t="n"/>
       <c r="AH27" s="2" t="n"/>
       <c r="AI27" s="2" t="n"/>
       <c r="AJ27" s="2" t="n"/>
@@ -3172,18 +3163,18 @@
         </is>
       </c>
       <c r="AC28" s="2" t="n"/>
-      <c r="AD28" s="19" t="inlineStr">
+      <c r="AD28" s="17" t="inlineStr">
         <is>
           <t>08:48</t>
         </is>
       </c>
-      <c r="AE28" s="19" t="n"/>
-      <c r="AF28" s="19" t="inlineStr">
+      <c r="AE28" s="2" t="n"/>
+      <c r="AF28" s="17" t="inlineStr">
         <is>
           <t>08:51</t>
         </is>
       </c>
-      <c r="AG28" s="19" t="n"/>
+      <c r="AG28" s="2" t="n"/>
       <c r="AH28" s="2" t="n"/>
       <c r="AI28" s="2" t="n"/>
       <c r="AJ28" s="2" t="n"/>
@@ -3288,18 +3279,18 @@
         </is>
       </c>
       <c r="AC29" s="2" t="n"/>
-      <c r="AD29" s="19" t="inlineStr">
+      <c r="AD29" s="17" t="inlineStr">
         <is>
           <t>17:40</t>
         </is>
       </c>
-      <c r="AE29" s="19" t="n"/>
-      <c r="AF29" s="19" t="inlineStr">
+      <c r="AE29" s="2" t="n"/>
+      <c r="AF29" s="17" t="inlineStr">
         <is>
           <t>17:07</t>
         </is>
       </c>
-      <c r="AG29" s="19" t="n"/>
+      <c r="AG29" s="2" t="n"/>
       <c r="AH29" s="2" t="n"/>
       <c r="AI29" s="2" t="n"/>
       <c r="AJ29" s="2" t="n"/>
@@ -3411,18 +3402,18 @@
         </is>
       </c>
       <c r="AC30" s="2" t="n"/>
-      <c r="AD30" s="19" t="inlineStr">
+      <c r="AD30" s="17" t="inlineStr">
         <is>
           <t>08:31</t>
         </is>
       </c>
-      <c r="AE30" s="19" t="n"/>
-      <c r="AF30" s="19" t="inlineStr">
+      <c r="AE30" s="2" t="n"/>
+      <c r="AF30" s="17" t="inlineStr">
         <is>
           <t>08:36</t>
         </is>
       </c>
-      <c r="AG30" s="19" t="n"/>
+      <c r="AG30" s="2" t="n"/>
       <c r="AH30" s="2" t="n"/>
       <c r="AI30" s="2" t="n"/>
       <c r="AJ30" s="2" t="n"/>
@@ -3523,18 +3514,18 @@
         </is>
       </c>
       <c r="AC31" s="2" t="n"/>
-      <c r="AD31" s="19" t="inlineStr">
+      <c r="AD31" s="17" t="inlineStr">
         <is>
           <t>16:41</t>
         </is>
       </c>
-      <c r="AE31" s="19" t="n"/>
-      <c r="AF31" s="19" t="inlineStr">
+      <c r="AE31" s="2" t="n"/>
+      <c r="AF31" s="17" t="inlineStr">
         <is>
           <t>16:44</t>
         </is>
       </c>
-      <c r="AG31" s="19" t="n"/>
+      <c r="AG31" s="2" t="n"/>
       <c r="AH31" s="2" t="n"/>
       <c r="AI31" s="2" t="n"/>
       <c r="AJ31" s="2" t="n"/>
@@ -4594,18 +4585,18 @@
         </is>
       </c>
       <c r="AC40" s="2" t="n"/>
-      <c r="AD40" s="19" t="inlineStr">
+      <c r="AD40" s="17" t="inlineStr">
         <is>
           <t>10:22</t>
         </is>
       </c>
-      <c r="AE40" s="19" t="n"/>
-      <c r="AF40" s="19" t="inlineStr">
+      <c r="AE40" s="2" t="n"/>
+      <c r="AF40" s="17" t="inlineStr">
         <is>
           <t>10:22</t>
         </is>
       </c>
-      <c r="AG40" s="19" t="n"/>
+      <c r="AG40" s="2" t="n"/>
       <c r="AH40" s="2" t="n"/>
       <c r="AI40" s="2" t="n"/>
       <c r="AJ40" s="2" t="n"/>
@@ -4710,18 +4701,18 @@
         </is>
       </c>
       <c r="AC41" s="2" t="n"/>
-      <c r="AD41" s="19" t="inlineStr">
+      <c r="AD41" s="17" t="inlineStr">
         <is>
           <t>17:03</t>
         </is>
       </c>
-      <c r="AE41" s="19" t="n"/>
-      <c r="AF41" s="19" t="inlineStr">
+      <c r="AE41" s="2" t="n"/>
+      <c r="AF41" s="17" t="inlineStr">
         <is>
           <t>17:31</t>
         </is>
       </c>
-      <c r="AG41" s="19" t="n"/>
+      <c r="AG41" s="2" t="n"/>
       <c r="AH41" s="2" t="n"/>
       <c r="AI41" s="2" t="n"/>
       <c r="AJ41" s="2" t="n"/>
@@ -5069,18 +5060,18 @@
         </is>
       </c>
       <c r="AC44" s="2" t="n"/>
-      <c r="AD44" s="19" t="inlineStr">
+      <c r="AD44" s="17" t="inlineStr">
         <is>
           <t>07:23</t>
         </is>
       </c>
-      <c r="AE44" s="19" t="n"/>
-      <c r="AF44" s="19" t="inlineStr">
+      <c r="AE44" s="2" t="n"/>
+      <c r="AF44" s="17" t="inlineStr">
         <is>
           <t>08:01</t>
         </is>
       </c>
-      <c r="AG44" s="19" t="n"/>
+      <c r="AG44" s="2" t="n"/>
       <c r="AH44" s="2" t="n"/>
       <c r="AI44" s="2" t="n"/>
       <c r="AJ44" s="2" t="n"/>
@@ -5185,18 +5176,18 @@
         </is>
       </c>
       <c r="AC45" s="2" t="n"/>
-      <c r="AD45" s="19" t="inlineStr">
+      <c r="AD45" s="17" t="inlineStr">
         <is>
           <t>18:39</t>
         </is>
       </c>
-      <c r="AE45" s="19" t="n"/>
-      <c r="AF45" s="19" t="inlineStr">
+      <c r="AE45" s="2" t="n"/>
+      <c r="AF45" s="17" t="inlineStr">
         <is>
           <t>17:45</t>
         </is>
       </c>
-      <c r="AG45" s="19" t="n"/>
+      <c r="AG45" s="2" t="n"/>
       <c r="AH45" s="2" t="n"/>
       <c r="AI45" s="2" t="n"/>
       <c r="AJ45" s="2" t="n"/>
@@ -5744,18 +5735,18 @@
         </is>
       </c>
       <c r="AC50" s="2" t="n"/>
-      <c r="AD50" s="19" t="inlineStr">
+      <c r="AD50" s="17" t="inlineStr">
         <is>
           <t>07:26</t>
         </is>
       </c>
-      <c r="AE50" s="19" t="n"/>
-      <c r="AF50" s="19" t="inlineStr">
+      <c r="AE50" s="2" t="n"/>
+      <c r="AF50" s="17" t="inlineStr">
         <is>
           <t>07:31</t>
         </is>
       </c>
-      <c r="AG50" s="19" t="n"/>
+      <c r="AG50" s="2" t="n"/>
       <c r="AH50" s="2" t="n"/>
       <c r="AI50" s="2" t="n"/>
       <c r="AJ50" s="2" t="n"/>
@@ -5860,18 +5851,18 @@
         </is>
       </c>
       <c r="AC51" s="2" t="n"/>
-      <c r="AD51" s="19" t="inlineStr">
+      <c r="AD51" s="17" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
-      <c r="AE51" s="19" t="n"/>
-      <c r="AF51" s="19" t="inlineStr">
+      <c r="AE51" s="2" t="n"/>
+      <c r="AF51" s="17" t="inlineStr">
         <is>
           <t>19:02</t>
         </is>
       </c>
-      <c r="AG51" s="19" t="n"/>
+      <c r="AG51" s="2" t="n"/>
       <c r="AH51" s="2" t="n"/>
       <c r="AI51" s="2" t="n"/>
       <c r="AJ51" s="2" t="n"/>
@@ -5987,18 +5978,18 @@
         </is>
       </c>
       <c r="AC52" s="2" t="n"/>
-      <c r="AD52" s="19" t="inlineStr">
+      <c r="AD52" s="17" t="inlineStr">
         <is>
           <t>08:34</t>
         </is>
       </c>
-      <c r="AE52" s="19" t="n"/>
-      <c r="AF52" s="19" t="inlineStr">
+      <c r="AE52" s="2" t="n"/>
+      <c r="AF52" s="17" t="inlineStr">
         <is>
           <t>08:27</t>
         </is>
       </c>
-      <c r="AG52" s="19" t="n"/>
+      <c r="AG52" s="2" t="n"/>
       <c r="AH52" s="2" t="n"/>
       <c r="AI52" s="2" t="n"/>
       <c r="AJ52" s="2" t="n"/>
@@ -6103,18 +6094,18 @@
         </is>
       </c>
       <c r="AC53" s="2" t="n"/>
-      <c r="AD53" s="19" t="inlineStr">
+      <c r="AD53" s="17" t="inlineStr">
         <is>
           <t>17:45</t>
         </is>
       </c>
-      <c r="AE53" s="19" t="n"/>
-      <c r="AF53" s="19" t="inlineStr">
+      <c r="AE53" s="2" t="n"/>
+      <c r="AF53" s="17" t="inlineStr">
         <is>
           <t>17:55</t>
         </is>
       </c>
-      <c r="AG53" s="19" t="n"/>
+      <c r="AG53" s="2" t="n"/>
       <c r="AH53" s="2" t="n"/>
       <c r="AI53" s="2" t="n"/>
       <c r="AJ53" s="2" t="n"/>
@@ -6230,18 +6221,18 @@
         </is>
       </c>
       <c r="AC54" s="2" t="n"/>
-      <c r="AD54" s="19" t="inlineStr">
+      <c r="AD54" s="17" t="inlineStr">
         <is>
           <t>08:34</t>
         </is>
       </c>
-      <c r="AE54" s="19" t="n"/>
-      <c r="AF54" s="19" t="inlineStr">
+      <c r="AE54" s="2" t="n"/>
+      <c r="AF54" s="17" t="inlineStr">
         <is>
           <t>08:40</t>
         </is>
       </c>
-      <c r="AG54" s="19" t="n"/>
+      <c r="AG54" s="2" t="n"/>
       <c r="AH54" s="2" t="n"/>
       <c r="AI54" s="2" t="n"/>
       <c r="AJ54" s="2" t="n"/>
@@ -6346,18 +6337,18 @@
         </is>
       </c>
       <c r="AC55" s="2" t="n"/>
-      <c r="AD55" s="19" t="inlineStr">
+      <c r="AD55" s="17" t="inlineStr">
         <is>
           <t>17:23</t>
         </is>
       </c>
-      <c r="AE55" s="19" t="n"/>
-      <c r="AF55" s="19" t="inlineStr">
+      <c r="AE55" s="2" t="n"/>
+      <c r="AF55" s="17" t="inlineStr">
         <is>
           <t>17:36</t>
         </is>
       </c>
-      <c r="AG55" s="19" t="n"/>
+      <c r="AG55" s="2" t="n"/>
       <c r="AH55" s="2" t="n"/>
       <c r="AI55" s="2" t="n"/>
       <c r="AJ55" s="2" t="n"/>
@@ -6465,12 +6456,12 @@
         </is>
       </c>
       <c r="AC56" s="2" t="n"/>
-      <c r="AD56" s="19" t="inlineStr">
+      <c r="AD56" s="17" t="inlineStr">
         <is>
           <t>08:36</t>
         </is>
       </c>
-      <c r="AE56" s="19" t="n"/>
+      <c r="AE56" s="2" t="n"/>
       <c r="AF56" s="2" t="n"/>
       <c r="AG56" s="2" t="n"/>
       <c r="AH56" s="2" t="n"/>
@@ -6569,12 +6560,12 @@
         </is>
       </c>
       <c r="AC57" s="2" t="n"/>
-      <c r="AD57" s="19" t="inlineStr">
+      <c r="AD57" s="17" t="inlineStr">
         <is>
           <t>19:40</t>
         </is>
       </c>
-      <c r="AE57" s="19" t="n"/>
+      <c r="AE57" s="2" t="n"/>
       <c r="AF57" s="2" t="n"/>
       <c r="AG57" s="2" t="n"/>
       <c r="AH57" s="2" t="n"/>
@@ -6692,12 +6683,12 @@
         </is>
       </c>
       <c r="AC58" s="2" t="n"/>
-      <c r="AD58" s="19" t="inlineStr">
+      <c r="AD58" s="17" t="inlineStr">
         <is>
           <t>08:48</t>
         </is>
       </c>
-      <c r="AE58" s="19" t="n"/>
+      <c r="AE58" s="2" t="n"/>
       <c r="AF58" s="2" t="n"/>
       <c r="AG58" s="2" t="n"/>
       <c r="AH58" s="2" t="n"/>
@@ -6804,12 +6795,12 @@
         </is>
       </c>
       <c r="AC59" s="2" t="n"/>
-      <c r="AD59" s="19" t="inlineStr">
+      <c r="AD59" s="17" t="inlineStr">
         <is>
           <t>17:49</t>
         </is>
       </c>
-      <c r="AE59" s="19" t="n"/>
+      <c r="AE59" s="2" t="n"/>
       <c r="AF59" s="2" t="n"/>
       <c r="AG59" s="2" t="n"/>
       <c r="AH59" s="2" t="n"/>
@@ -7839,22 +7830,22 @@
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
       </c>
-      <c r="AD68" s="19" t="inlineStr">
+      <c r="AD68" s="17" t="inlineStr">
         <is>
           <t>08:18</t>
         </is>
       </c>
-      <c r="AE68" s="19" t="inlineStr">
+      <c r="AE68" s="2" t="inlineStr">
         <is>
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
       </c>
-      <c r="AF68" s="19" t="inlineStr">
+      <c r="AF68" s="17" t="inlineStr">
         <is>
           <t>08:00</t>
         </is>
       </c>
-      <c r="AG68" s="19" t="inlineStr">
+      <c r="AG68" s="2" t="inlineStr">
         <is>
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
@@ -7987,22 +7978,22 @@
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
       </c>
-      <c r="AD69" s="19" t="inlineStr">
+      <c r="AD69" s="17" t="inlineStr">
         <is>
           <t>15:13</t>
         </is>
       </c>
-      <c r="AE69" s="19" t="inlineStr">
+      <c r="AE69" s="2" t="inlineStr">
         <is>
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
       </c>
-      <c r="AF69" s="19" t="inlineStr">
+      <c r="AF69" s="17" t="inlineStr">
         <is>
           <t>14:50</t>
         </is>
       </c>
-      <c r="AG69" s="19" t="inlineStr">
+      <c r="AG69" s="2" t="inlineStr">
         <is>
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
@@ -8360,12 +8351,12 @@
       <c r="AC72" s="2" t="n"/>
       <c r="AD72" s="2" t="n"/>
       <c r="AE72" s="2" t="n"/>
-      <c r="AF72" s="19" t="inlineStr">
+      <c r="AF72" s="17" t="inlineStr">
         <is>
           <t>09:00</t>
         </is>
       </c>
-      <c r="AG72" s="19" t="n"/>
+      <c r="AG72" s="2" t="n"/>
       <c r="AH72" s="2" t="n"/>
       <c r="AI72" s="2" t="n"/>
       <c r="AJ72" s="2" t="n"/>
@@ -8468,12 +8459,12 @@
       <c r="AC73" s="2" t="n"/>
       <c r="AD73" s="2" t="n"/>
       <c r="AE73" s="2" t="n"/>
-      <c r="AF73" s="19" t="inlineStr">
+      <c r="AF73" s="17" t="inlineStr">
         <is>
           <t>17:28</t>
         </is>
       </c>
-      <c r="AG73" s="19" t="n"/>
+      <c r="AG73" s="2" t="n"/>
       <c r="AH73" s="2" t="n"/>
       <c r="AI73" s="2" t="n"/>
       <c r="AJ73" s="2" t="n"/>
@@ -8589,18 +8580,18 @@
         </is>
       </c>
       <c r="AC74" s="2" t="n"/>
-      <c r="AD74" s="19" t="inlineStr">
+      <c r="AD74" s="17" t="inlineStr">
         <is>
           <t>09:25</t>
         </is>
       </c>
-      <c r="AE74" s="19" t="n"/>
-      <c r="AF74" s="19" t="inlineStr">
+      <c r="AE74" s="2" t="n"/>
+      <c r="AF74" s="17" t="inlineStr">
         <is>
           <t>08:57</t>
         </is>
       </c>
-      <c r="AG74" s="19" t="n"/>
+      <c r="AG74" s="2" t="n"/>
       <c r="AH74" s="2" t="n"/>
       <c r="AI74" s="2" t="n"/>
       <c r="AJ74" s="2" t="n"/>
@@ -8705,18 +8696,18 @@
         </is>
       </c>
       <c r="AC75" s="2" t="n"/>
-      <c r="AD75" s="19" t="inlineStr">
+      <c r="AD75" s="17" t="inlineStr">
         <is>
           <t>17:35</t>
         </is>
       </c>
-      <c r="AE75" s="19" t="n"/>
-      <c r="AF75" s="19" t="inlineStr">
+      <c r="AE75" s="2" t="n"/>
+      <c r="AF75" s="17" t="inlineStr">
         <is>
           <t>18:23</t>
         </is>
       </c>
-      <c r="AG75" s="19" t="n"/>
+      <c r="AG75" s="2" t="n"/>
       <c r="AH75" s="2" t="n"/>
       <c r="AI75" s="2" t="n"/>
       <c r="AJ75" s="2" t="n"/>
@@ -8832,18 +8823,18 @@
         </is>
       </c>
       <c r="AC76" s="2" t="n"/>
-      <c r="AD76" s="19" t="inlineStr">
+      <c r="AD76" s="17" t="inlineStr">
         <is>
           <t>08:08</t>
         </is>
       </c>
-      <c r="AE76" s="19" t="n"/>
-      <c r="AF76" s="19" t="inlineStr">
+      <c r="AE76" s="2" t="n"/>
+      <c r="AF76" s="17" t="inlineStr">
         <is>
           <t>08:35</t>
         </is>
       </c>
-      <c r="AG76" s="19" t="n"/>
+      <c r="AG76" s="2" t="n"/>
       <c r="AH76" s="2" t="n"/>
       <c r="AI76" s="2" t="n"/>
       <c r="AJ76" s="2" t="n"/>
@@ -8948,18 +8939,18 @@
         </is>
       </c>
       <c r="AC77" s="2" t="n"/>
-      <c r="AD77" s="19" t="inlineStr">
+      <c r="AD77" s="17" t="inlineStr">
         <is>
           <t>16:42</t>
         </is>
       </c>
-      <c r="AE77" s="19" t="n"/>
-      <c r="AF77" s="19" t="inlineStr">
+      <c r="AE77" s="2" t="n"/>
+      <c r="AF77" s="17" t="inlineStr">
         <is>
           <t>17:44</t>
         </is>
       </c>
-      <c r="AG77" s="19" t="n"/>
+      <c r="AG77" s="2" t="n"/>
       <c r="AH77" s="2" t="n"/>
       <c r="AI77" s="2" t="n"/>
       <c r="AJ77" s="2" t="n"/>
@@ -9075,18 +9066,18 @@
         </is>
       </c>
       <c r="AC78" s="2" t="n"/>
-      <c r="AD78" s="19" t="inlineStr">
+      <c r="AD78" s="17" t="inlineStr">
         <is>
           <t>09:11</t>
         </is>
       </c>
-      <c r="AE78" s="19" t="n"/>
-      <c r="AF78" s="19" t="inlineStr">
+      <c r="AE78" s="2" t="n"/>
+      <c r="AF78" s="17" t="inlineStr">
         <is>
           <t>09:26</t>
         </is>
       </c>
-      <c r="AG78" s="19" t="n"/>
+      <c r="AG78" s="2" t="n"/>
       <c r="AH78" s="2" t="n"/>
       <c r="AI78" s="2" t="n"/>
       <c r="AJ78" s="2" t="n"/>
@@ -9191,18 +9182,18 @@
         </is>
       </c>
       <c r="AC79" s="2" t="n"/>
-      <c r="AD79" s="19" t="inlineStr">
+      <c r="AD79" s="17" t="inlineStr">
         <is>
           <t>16:37</t>
         </is>
       </c>
-      <c r="AE79" s="19" t="n"/>
-      <c r="AF79" s="19" t="inlineStr">
+      <c r="AE79" s="2" t="n"/>
+      <c r="AF79" s="17" t="inlineStr">
         <is>
           <t>18:10</t>
         </is>
       </c>
-      <c r="AG79" s="19" t="n"/>
+      <c r="AG79" s="2" t="n"/>
       <c r="AH79" s="2" t="n"/>
       <c r="AI79" s="2" t="n"/>
       <c r="AJ79" s="2" t="n"/>
@@ -9736,12 +9727,12 @@
       <c r="AC84" s="2" t="n"/>
       <c r="AD84" s="2" t="n"/>
       <c r="AE84" s="2" t="n"/>
-      <c r="AF84" s="19" t="inlineStr">
+      <c r="AF84" s="17" t="inlineStr">
         <is>
           <t>10:24</t>
         </is>
       </c>
-      <c r="AG84" s="19" t="n"/>
+      <c r="AG84" s="2" t="n"/>
       <c r="AH84" s="2" t="n"/>
       <c r="AI84" s="2" t="n"/>
       <c r="AJ84" s="2" t="n"/>
@@ -9848,12 +9839,12 @@
       <c r="AC85" s="2" t="n"/>
       <c r="AD85" s="2" t="n"/>
       <c r="AE85" s="2" t="n"/>
-      <c r="AF85" s="19" t="inlineStr">
+      <c r="AF85" s="17" t="inlineStr">
         <is>
           <t>17:46</t>
         </is>
       </c>
-      <c r="AG85" s="19" t="n"/>
+      <c r="AG85" s="2" t="n"/>
       <c r="AH85" s="2" t="n"/>
       <c r="AI85" s="2" t="n"/>
       <c r="AJ85" s="2" t="n"/>
@@ -9965,18 +9956,18 @@
       <c r="AA86" s="2" t="n"/>
       <c r="AB86" s="2" t="n"/>
       <c r="AC86" s="2" t="n"/>
-      <c r="AD86" s="19" t="inlineStr">
+      <c r="AD86" s="17" t="inlineStr">
         <is>
           <t>10:15</t>
         </is>
       </c>
-      <c r="AE86" s="19" t="n"/>
-      <c r="AF86" s="19" t="inlineStr">
+      <c r="AE86" s="2" t="n"/>
+      <c r="AF86" s="17" t="inlineStr">
         <is>
           <t>08:51</t>
         </is>
       </c>
-      <c r="AG86" s="19" t="n"/>
+      <c r="AG86" s="2" t="n"/>
       <c r="AH86" s="2" t="n"/>
       <c r="AI86" s="2" t="n"/>
       <c r="AJ86" s="2" t="n"/>
@@ -10077,18 +10068,18 @@
       <c r="AA87" s="2" t="n"/>
       <c r="AB87" s="2" t="n"/>
       <c r="AC87" s="2" t="n"/>
-      <c r="AD87" s="19" t="inlineStr">
+      <c r="AD87" s="17" t="inlineStr">
         <is>
           <t>17:17</t>
         </is>
       </c>
-      <c r="AE87" s="19" t="n"/>
-      <c r="AF87" s="19" t="inlineStr">
+      <c r="AE87" s="2" t="n"/>
+      <c r="AF87" s="17" t="inlineStr">
         <is>
           <t>16:07</t>
         </is>
       </c>
-      <c r="AG87" s="19" t="n"/>
+      <c r="AG87" s="2" t="n"/>
       <c r="AH87" s="2" t="n"/>
       <c r="AI87" s="2" t="n"/>
       <c r="AJ87" s="2" t="n"/>
@@ -10204,18 +10195,18 @@
         </is>
       </c>
       <c r="AC88" s="2" t="n"/>
-      <c r="AD88" s="19" t="inlineStr">
+      <c r="AD88" s="17" t="inlineStr">
         <is>
           <t>08:54</t>
         </is>
       </c>
-      <c r="AE88" s="19" t="n"/>
-      <c r="AF88" s="19" t="inlineStr">
+      <c r="AE88" s="2" t="n"/>
+      <c r="AF88" s="17" t="inlineStr">
         <is>
           <t>08:48</t>
         </is>
       </c>
-      <c r="AG88" s="19" t="n"/>
+      <c r="AG88" s="2" t="n"/>
       <c r="AH88" s="2" t="n"/>
       <c r="AI88" s="2" t="n"/>
       <c r="AJ88" s="2" t="n"/>
@@ -10316,18 +10307,18 @@
         </is>
       </c>
       <c r="AC89" s="2" t="n"/>
-      <c r="AD89" s="19" t="inlineStr">
+      <c r="AD89" s="17" t="inlineStr">
         <is>
           <t>18:48</t>
         </is>
       </c>
-      <c r="AE89" s="19" t="n"/>
-      <c r="AF89" s="19" t="inlineStr">
+      <c r="AE89" s="2" t="n"/>
+      <c r="AF89" s="17" t="inlineStr">
         <is>
           <t>18:41</t>
         </is>
       </c>
-      <c r="AG89" s="19" t="n"/>
+      <c r="AG89" s="2" t="n"/>
       <c r="AH89" s="2" t="n"/>
       <c r="AI89" s="2" t="n"/>
       <c r="AJ89" s="2" t="n"/>
@@ -10443,12 +10434,12 @@
         </is>
       </c>
       <c r="AC90" s="2" t="n"/>
-      <c r="AD90" s="19" t="inlineStr">
+      <c r="AD90" s="17" t="inlineStr">
         <is>
           <t>07:36</t>
         </is>
       </c>
-      <c r="AE90" s="19" t="n"/>
+      <c r="AE90" s="2" t="n"/>
       <c r="AF90" s="2" t="inlineStr">
         <is>
           <t>07:31</t>
@@ -10559,12 +10550,12 @@
         </is>
       </c>
       <c r="AC91" s="2" t="n"/>
-      <c r="AD91" s="19" t="inlineStr">
+      <c r="AD91" s="17" t="inlineStr">
         <is>
           <t>16:55</t>
         </is>
       </c>
-      <c r="AE91" s="19" t="n"/>
+      <c r="AE91" s="2" t="n"/>
       <c r="AF91" s="2" t="inlineStr">
         <is>
           <t>13:15</t>
@@ -10686,18 +10677,18 @@
         </is>
       </c>
       <c r="AC92" s="2" t="n"/>
-      <c r="AD92" s="19" t="inlineStr">
+      <c r="AD92" s="17" t="inlineStr">
         <is>
           <t>08:32</t>
         </is>
       </c>
-      <c r="AE92" s="19" t="n"/>
-      <c r="AF92" s="19" t="inlineStr">
+      <c r="AE92" s="2" t="n"/>
+      <c r="AF92" s="17" t="inlineStr">
         <is>
           <t>08:41</t>
         </is>
       </c>
-      <c r="AG92" s="19" t="n"/>
+      <c r="AG92" s="2" t="n"/>
       <c r="AH92" s="2" t="n"/>
       <c r="AI92" s="2" t="n"/>
       <c r="AJ92" s="2" t="n"/>
@@ -10802,18 +10793,18 @@
         </is>
       </c>
       <c r="AC93" s="2" t="n"/>
-      <c r="AD93" s="19" t="inlineStr">
+      <c r="AD93" s="17" t="inlineStr">
         <is>
           <t>17:22</t>
         </is>
       </c>
-      <c r="AE93" s="19" t="n"/>
-      <c r="AF93" s="19" t="inlineStr">
+      <c r="AE93" s="2" t="n"/>
+      <c r="AF93" s="17" t="inlineStr">
         <is>
           <t>18:37</t>
         </is>
       </c>
-      <c r="AG93" s="19" t="n"/>
+      <c r="AG93" s="2" t="n"/>
       <c r="AH93" s="2" t="n"/>
       <c r="AI93" s="2" t="n"/>
       <c r="AJ93" s="2" t="n"/>
@@ -10929,18 +10920,18 @@
         </is>
       </c>
       <c r="AC94" s="2" t="n"/>
-      <c r="AD94" s="19" t="inlineStr">
+      <c r="AD94" s="17" t="inlineStr">
         <is>
           <t>07:20</t>
         </is>
       </c>
-      <c r="AE94" s="19" t="n"/>
-      <c r="AF94" s="19" t="inlineStr">
+      <c r="AE94" s="2" t="n"/>
+      <c r="AF94" s="17" t="inlineStr">
         <is>
           <t>07:45</t>
         </is>
       </c>
-      <c r="AG94" s="19" t="n"/>
+      <c r="AG94" s="2" t="n"/>
       <c r="AH94" s="2" t="n"/>
       <c r="AI94" s="2" t="n"/>
       <c r="AJ94" s="2" t="n"/>
@@ -11045,18 +11036,18 @@
         </is>
       </c>
       <c r="AC95" s="2" t="n"/>
-      <c r="AD95" s="19" t="inlineStr">
+      <c r="AD95" s="17" t="inlineStr">
         <is>
           <t>17:47</t>
         </is>
       </c>
-      <c r="AE95" s="19" t="n"/>
-      <c r="AF95" s="19" t="inlineStr">
+      <c r="AE95" s="2" t="n"/>
+      <c r="AF95" s="17" t="inlineStr">
         <is>
           <t>17:39</t>
         </is>
       </c>
-      <c r="AG95" s="19" t="n"/>
+      <c r="AG95" s="2" t="n"/>
       <c r="AH95" s="2" t="n"/>
       <c r="AI95" s="2" t="n"/>
       <c r="AJ95" s="2" t="n"/>
@@ -11658,12 +11649,12 @@
         </is>
       </c>
       <c r="AE100" s="2" t="n"/>
-      <c r="AF100" s="19" t="inlineStr">
+      <c r="AF100" s="17" t="inlineStr">
         <is>
           <t>07:31</t>
         </is>
       </c>
-      <c r="AG100" s="19" t="n"/>
+      <c r="AG100" s="2" t="n"/>
       <c r="AH100" s="2" t="n"/>
       <c r="AI100" s="2" t="n"/>
       <c r="AJ100" s="2" t="n"/>
@@ -11774,12 +11765,12 @@
         </is>
       </c>
       <c r="AE101" s="2" t="n"/>
-      <c r="AF101" s="19" t="inlineStr">
+      <c r="AF101" s="17" t="inlineStr">
         <is>
           <t>15:29</t>
         </is>
       </c>
-      <c r="AG101" s="19" t="n"/>
+      <c r="AG101" s="2" t="n"/>
       <c r="AH101" s="2" t="n"/>
       <c r="AI101" s="2" t="n"/>
       <c r="AJ101" s="2" t="n"/>
@@ -12167,18 +12158,18 @@
         </is>
       </c>
       <c r="AC104" s="2" t="n"/>
-      <c r="AD104" s="19" t="inlineStr">
+      <c r="AD104" s="17" t="inlineStr">
         <is>
           <t>09:16</t>
         </is>
       </c>
-      <c r="AE104" s="19" t="n"/>
-      <c r="AF104" s="19" t="inlineStr">
+      <c r="AE104" s="2" t="n"/>
+      <c r="AF104" s="17" t="inlineStr">
         <is>
           <t>08:53</t>
         </is>
       </c>
-      <c r="AG104" s="19" t="n"/>
+      <c r="AG104" s="2" t="n"/>
       <c r="AH104" s="2" t="n"/>
       <c r="AI104" s="2" t="n"/>
       <c r="AJ104" s="2" t="n"/>
@@ -12283,18 +12274,18 @@
         </is>
       </c>
       <c r="AC105" s="2" t="n"/>
-      <c r="AD105" s="19" t="inlineStr">
+      <c r="AD105" s="17" t="inlineStr">
         <is>
           <t>17:36</t>
         </is>
       </c>
-      <c r="AE105" s="19" t="n"/>
-      <c r="AF105" s="19" t="inlineStr">
+      <c r="AE105" s="2" t="n"/>
+      <c r="AF105" s="17" t="inlineStr">
         <is>
           <t>17:01</t>
         </is>
       </c>
-      <c r="AG105" s="19" t="n"/>
+      <c r="AG105" s="2" t="n"/>
       <c r="AH105" s="2" t="n"/>
       <c r="AI105" s="2" t="n"/>
       <c r="AJ105" s="2" t="n"/>
@@ -12402,18 +12393,18 @@
       <c r="AA106" s="2" t="n"/>
       <c r="AB106" s="2" t="n"/>
       <c r="AC106" s="2" t="n"/>
-      <c r="AD106" s="19" t="inlineStr">
+      <c r="AD106" s="17" t="inlineStr">
         <is>
           <t>08:12</t>
         </is>
       </c>
-      <c r="AE106" s="19" t="n"/>
-      <c r="AF106" s="19" t="inlineStr">
+      <c r="AE106" s="2" t="n"/>
+      <c r="AF106" s="17" t="inlineStr">
         <is>
           <t>07:52</t>
         </is>
       </c>
-      <c r="AG106" s="19" t="n"/>
+      <c r="AG106" s="2" t="n"/>
       <c r="AH106" s="2" t="n"/>
       <c r="AI106" s="2" t="n"/>
       <c r="AJ106" s="2" t="n"/>
@@ -12510,18 +12501,18 @@
       <c r="AA107" s="2" t="n"/>
       <c r="AB107" s="2" t="n"/>
       <c r="AC107" s="2" t="n"/>
-      <c r="AD107" s="19" t="inlineStr">
+      <c r="AD107" s="17" t="inlineStr">
         <is>
           <t>17:45</t>
         </is>
       </c>
-      <c r="AE107" s="19" t="n"/>
-      <c r="AF107" s="19" t="inlineStr">
+      <c r="AE107" s="2" t="n"/>
+      <c r="AF107" s="17" t="inlineStr">
         <is>
           <t>18:30</t>
         </is>
       </c>
-      <c r="AG107" s="19" t="n"/>
+      <c r="AG107" s="2" t="n"/>
       <c r="AH107" s="2" t="n"/>
       <c r="AI107" s="2" t="n"/>
       <c r="AJ107" s="2" t="n"/>
@@ -12639,12 +12630,12 @@
         </is>
       </c>
       <c r="AE108" s="2" t="n"/>
-      <c r="AF108" s="19" t="inlineStr">
+      <c r="AF108" s="17" t="inlineStr">
         <is>
           <t>07:48</t>
         </is>
       </c>
-      <c r="AG108" s="19" t="n"/>
+      <c r="AG108" s="2" t="n"/>
       <c r="AH108" s="2" t="n"/>
       <c r="AI108" s="2" t="n"/>
       <c r="AJ108" s="2" t="n"/>
@@ -12751,12 +12742,12 @@
         </is>
       </c>
       <c r="AE109" s="2" t="n"/>
-      <c r="AF109" s="19" t="inlineStr">
+      <c r="AF109" s="17" t="inlineStr">
         <is>
           <t>18:01</t>
         </is>
       </c>
-      <c r="AG109" s="19" t="n"/>
+      <c r="AG109" s="2" t="n"/>
       <c r="AH109" s="2" t="n"/>
       <c r="AI109" s="2" t="n"/>
       <c r="AJ109" s="2" t="n"/>
@@ -12868,18 +12859,18 @@
         </is>
       </c>
       <c r="AC110" s="2" t="n"/>
-      <c r="AD110" s="19" t="inlineStr">
+      <c r="AD110" s="17" t="inlineStr">
         <is>
           <t>07:40</t>
         </is>
       </c>
-      <c r="AE110" s="19" t="n"/>
-      <c r="AF110" s="19" t="inlineStr">
+      <c r="AE110" s="2" t="n"/>
+      <c r="AF110" s="17" t="inlineStr">
         <is>
           <t>07:44</t>
         </is>
       </c>
-      <c r="AG110" s="19" t="n"/>
+      <c r="AG110" s="2" t="n"/>
       <c r="AH110" s="2" t="n"/>
       <c r="AI110" s="2" t="n"/>
       <c r="AJ110" s="2" t="n"/>
@@ -12980,18 +12971,18 @@
         </is>
       </c>
       <c r="AC111" s="2" t="n"/>
-      <c r="AD111" s="19" t="inlineStr">
+      <c r="AD111" s="17" t="inlineStr">
         <is>
           <t>18:00</t>
         </is>
       </c>
-      <c r="AE111" s="19" t="n"/>
-      <c r="AF111" s="19" t="inlineStr">
+      <c r="AE111" s="2" t="n"/>
+      <c r="AF111" s="17" t="inlineStr">
         <is>
           <t>18:35</t>
         </is>
       </c>
-      <c r="AG111" s="19" t="n"/>
+      <c r="AG111" s="2" t="n"/>
       <c r="AH111" s="2" t="n"/>
       <c r="AI111" s="2" t="n"/>
       <c r="AJ111" s="2" t="n"/>
@@ -13103,12 +13094,12 @@
         </is>
       </c>
       <c r="AC112" s="2" t="n"/>
-      <c r="AD112" s="19" t="inlineStr">
+      <c r="AD112" s="17" t="inlineStr">
         <is>
           <t>07:44</t>
         </is>
       </c>
-      <c r="AE112" s="19" t="n"/>
+      <c r="AE112" s="2" t="n"/>
       <c r="AF112" s="2" t="inlineStr">
         <is>
           <t>07:45</t>
@@ -13215,12 +13206,12 @@
         </is>
       </c>
       <c r="AC113" s="2" t="n"/>
-      <c r="AD113" s="19" t="inlineStr">
+      <c r="AD113" s="17" t="inlineStr">
         <is>
           <t>17:36</t>
         </is>
       </c>
-      <c r="AE113" s="19" t="n"/>
+      <c r="AE113" s="2" t="n"/>
       <c r="AF113" s="2" t="inlineStr">
         <is>
           <t>13:15</t>
@@ -13330,18 +13321,18 @@
       <c r="AA114" s="2" t="n"/>
       <c r="AB114" s="2" t="n"/>
       <c r="AC114" s="2" t="n"/>
-      <c r="AD114" s="19" t="inlineStr">
+      <c r="AD114" s="17" t="inlineStr">
         <is>
           <t>07:20</t>
         </is>
       </c>
-      <c r="AE114" s="19" t="n"/>
-      <c r="AF114" s="19" t="inlineStr">
+      <c r="AE114" s="2" t="n"/>
+      <c r="AF114" s="17" t="inlineStr">
         <is>
           <t>07:44</t>
         </is>
       </c>
-      <c r="AG114" s="19" t="n"/>
+      <c r="AG114" s="2" t="n"/>
       <c r="AH114" s="2" t="n"/>
       <c r="AI114" s="2" t="n"/>
       <c r="AJ114" s="2" t="n"/>
@@ -13434,18 +13425,18 @@
       <c r="AA115" s="2" t="n"/>
       <c r="AB115" s="2" t="n"/>
       <c r="AC115" s="2" t="n"/>
-      <c r="AD115" s="19" t="inlineStr">
+      <c r="AD115" s="17" t="inlineStr">
         <is>
           <t>16:37</t>
         </is>
       </c>
-      <c r="AE115" s="19" t="n"/>
-      <c r="AF115" s="19" t="inlineStr">
+      <c r="AE115" s="2" t="n"/>
+      <c r="AF115" s="17" t="inlineStr">
         <is>
           <t>17:49</t>
         </is>
       </c>
-      <c r="AG115" s="19" t="n"/>
+      <c r="AG115" s="2" t="n"/>
       <c r="AH115" s="2" t="n"/>
       <c r="AI115" s="2" t="n"/>
       <c r="AJ115" s="2" t="n"/>
@@ -13561,18 +13552,18 @@
         </is>
       </c>
       <c r="AC116" s="2" t="n"/>
-      <c r="AD116" s="19" t="inlineStr">
+      <c r="AD116" s="17" t="inlineStr">
         <is>
           <t>07:38</t>
         </is>
       </c>
-      <c r="AE116" s="19" t="n"/>
-      <c r="AF116" s="19" t="inlineStr">
+      <c r="AE116" s="2" t="n"/>
+      <c r="AF116" s="17" t="inlineStr">
         <is>
           <t>07:44</t>
         </is>
       </c>
-      <c r="AG116" s="19" t="n"/>
+      <c r="AG116" s="2" t="n"/>
       <c r="AH116" s="2" t="n"/>
       <c r="AI116" s="2" t="n"/>
       <c r="AJ116" s="2" t="n"/>
@@ -13677,18 +13668,18 @@
         </is>
       </c>
       <c r="AC117" s="2" t="n"/>
-      <c r="AD117" s="19" t="inlineStr">
+      <c r="AD117" s="17" t="inlineStr">
         <is>
           <t>17:17</t>
         </is>
       </c>
-      <c r="AE117" s="19" t="n"/>
-      <c r="AF117" s="19" t="inlineStr">
+      <c r="AE117" s="2" t="n"/>
+      <c r="AF117" s="17" t="inlineStr">
         <is>
           <t>17:45</t>
         </is>
       </c>
-      <c r="AG117" s="19" t="n"/>
+      <c r="AG117" s="2" t="n"/>
       <c r="AH117" s="2" t="n"/>
       <c r="AI117" s="2" t="n"/>
       <c r="AJ117" s="2" t="n"/>
@@ -14252,18 +14243,18 @@
         </is>
       </c>
       <c r="AC122" s="2" t="n"/>
-      <c r="AD122" s="19" t="inlineStr">
+      <c r="AD122" s="17" t="inlineStr">
         <is>
           <t>08:08</t>
         </is>
       </c>
-      <c r="AE122" s="19" t="n"/>
-      <c r="AF122" s="19" t="inlineStr">
+      <c r="AE122" s="2" t="n"/>
+      <c r="AF122" s="17" t="inlineStr">
         <is>
           <t>08:35</t>
         </is>
       </c>
-      <c r="AG122" s="19" t="n"/>
+      <c r="AG122" s="2" t="n"/>
       <c r="AH122" s="2" t="n"/>
       <c r="AI122" s="2" t="n"/>
       <c r="AJ122" s="2" t="n"/>
@@ -14368,18 +14359,18 @@
         </is>
       </c>
       <c r="AC123" s="2" t="n"/>
-      <c r="AD123" s="19" t="inlineStr">
+      <c r="AD123" s="17" t="inlineStr">
         <is>
           <t>16:42</t>
         </is>
       </c>
-      <c r="AE123" s="19" t="n"/>
-      <c r="AF123" s="19" t="inlineStr">
+      <c r="AE123" s="2" t="n"/>
+      <c r="AF123" s="17" t="inlineStr">
         <is>
           <t>17:45</t>
         </is>
       </c>
-      <c r="AG123" s="19" t="n"/>
+      <c r="AG123" s="2" t="n"/>
       <c r="AH123" s="2" t="n"/>
       <c r="AI123" s="2" t="n"/>
       <c r="AJ123" s="2" t="n"/>
@@ -14707,18 +14698,18 @@
         </is>
       </c>
       <c r="AC126" s="2" t="n"/>
-      <c r="AD126" s="19" t="inlineStr">
+      <c r="AD126" s="17" t="inlineStr">
         <is>
           <t>07:32</t>
         </is>
       </c>
-      <c r="AE126" s="19" t="n"/>
-      <c r="AF126" s="19" t="inlineStr">
+      <c r="AE126" s="2" t="n"/>
+      <c r="AF126" s="17" t="inlineStr">
         <is>
           <t>07:45</t>
         </is>
       </c>
-      <c r="AG126" s="19" t="n"/>
+      <c r="AG126" s="2" t="n"/>
       <c r="AH126" s="2" t="n"/>
       <c r="AI126" s="2" t="n"/>
       <c r="AJ126" s="2" t="n"/>
@@ -14819,18 +14810,18 @@
         </is>
       </c>
       <c r="AC127" s="2" t="n"/>
-      <c r="AD127" s="19" t="inlineStr">
+      <c r="AD127" s="17" t="inlineStr">
         <is>
           <t>18:29</t>
         </is>
       </c>
-      <c r="AE127" s="19" t="n"/>
-      <c r="AF127" s="19" t="inlineStr">
+      <c r="AE127" s="2" t="n"/>
+      <c r="AF127" s="17" t="inlineStr">
         <is>
           <t>18:20</t>
         </is>
       </c>
-      <c r="AG127" s="19" t="n"/>
+      <c r="AG127" s="2" t="n"/>
       <c r="AH127" s="2" t="n"/>
       <c r="AI127" s="2" t="n"/>
       <c r="AJ127" s="2" t="n"/>
@@ -15162,18 +15153,18 @@
         </is>
       </c>
       <c r="AC130" s="2" t="n"/>
-      <c r="AD130" s="19" t="inlineStr">
+      <c r="AD130" s="17" t="inlineStr">
         <is>
           <t>08:34</t>
         </is>
       </c>
-      <c r="AE130" s="19" t="n"/>
-      <c r="AF130" s="19" t="inlineStr">
+      <c r="AE130" s="2" t="n"/>
+      <c r="AF130" s="17" t="inlineStr">
         <is>
           <t>08:40</t>
         </is>
       </c>
-      <c r="AG130" s="19" t="n"/>
+      <c r="AG130" s="2" t="n"/>
       <c r="AH130" s="2" t="n"/>
       <c r="AI130" s="2" t="n"/>
       <c r="AJ130" s="2" t="n"/>
@@ -15278,18 +15269,18 @@
         </is>
       </c>
       <c r="AC131" s="2" t="n"/>
-      <c r="AD131" s="19" t="inlineStr">
+      <c r="AD131" s="17" t="inlineStr">
         <is>
           <t>17:23</t>
         </is>
       </c>
-      <c r="AE131" s="19" t="n"/>
-      <c r="AF131" s="19" t="inlineStr">
+      <c r="AE131" s="2" t="n"/>
+      <c r="AF131" s="17" t="inlineStr">
         <is>
           <t>17:36</t>
         </is>
       </c>
-      <c r="AG131" s="19" t="n"/>
+      <c r="AG131" s="2" t="n"/>
       <c r="AH131" s="2" t="n"/>
       <c r="AI131" s="2" t="n"/>
       <c r="AJ131" s="2" t="n"/>
@@ -15397,18 +15388,18 @@
         </is>
       </c>
       <c r="AC132" s="2" t="n"/>
-      <c r="AD132" s="19" t="inlineStr">
+      <c r="AD132" s="17" t="inlineStr">
         <is>
           <t>07:40</t>
         </is>
       </c>
-      <c r="AE132" s="19" t="n"/>
-      <c r="AF132" s="19" t="inlineStr">
+      <c r="AE132" s="2" t="n"/>
+      <c r="AF132" s="17" t="inlineStr">
         <is>
           <t>07:44</t>
         </is>
       </c>
-      <c r="AG132" s="19" t="n"/>
+      <c r="AG132" s="2" t="n"/>
       <c r="AH132" s="2" t="n"/>
       <c r="AI132" s="2" t="n"/>
       <c r="AJ132" s="2" t="n"/>
@@ -15505,18 +15496,18 @@
         </is>
       </c>
       <c r="AC133" s="2" t="n"/>
-      <c r="AD133" s="19" t="inlineStr">
+      <c r="AD133" s="17" t="inlineStr">
         <is>
           <t>18:14</t>
         </is>
       </c>
-      <c r="AE133" s="19" t="n"/>
-      <c r="AF133" s="19" t="inlineStr">
+      <c r="AE133" s="2" t="n"/>
+      <c r="AF133" s="17" t="inlineStr">
         <is>
           <t>18:56</t>
         </is>
       </c>
-      <c r="AG133" s="19" t="n"/>
+      <c r="AG133" s="2" t="n"/>
       <c r="AH133" s="2" t="n"/>
       <c r="AI133" s="2" t="n"/>
       <c r="AJ133" s="2" t="n"/>
@@ -15634,12 +15625,12 @@
       <c r="AC134" s="2" t="n"/>
       <c r="AD134" s="2" t="n"/>
       <c r="AE134" s="2" t="n"/>
-      <c r="AF134" s="19" t="inlineStr">
+      <c r="AF134" s="17" t="inlineStr">
         <is>
           <t>08:55</t>
         </is>
       </c>
-      <c r="AG134" s="19" t="n"/>
+      <c r="AG134" s="2" t="n"/>
       <c r="AH134" s="2" t="n"/>
       <c r="AI134" s="2" t="n"/>
       <c r="AJ134" s="2" t="n"/>
@@ -15746,12 +15737,12 @@
       <c r="AC135" s="2" t="n"/>
       <c r="AD135" s="2" t="n"/>
       <c r="AE135" s="2" t="n"/>
-      <c r="AF135" s="19" t="inlineStr">
+      <c r="AF135" s="17" t="inlineStr">
         <is>
           <t>16:59</t>
         </is>
       </c>
-      <c r="AG135" s="19" t="n"/>
+      <c r="AG135" s="2" t="n"/>
       <c r="AH135" s="2" t="n"/>
       <c r="AI135" s="2" t="n"/>
       <c r="AJ135" s="2" t="n"/>
@@ -15867,18 +15858,18 @@
         </is>
       </c>
       <c r="AC136" s="2" t="n"/>
-      <c r="AD136" s="19" t="inlineStr">
+      <c r="AD136" s="17" t="inlineStr">
         <is>
           <t>08:49</t>
         </is>
       </c>
-      <c r="AE136" s="19" t="n"/>
-      <c r="AF136" s="19" t="inlineStr">
+      <c r="AE136" s="2" t="n"/>
+      <c r="AF136" s="17" t="inlineStr">
         <is>
           <t>08:50</t>
         </is>
       </c>
-      <c r="AG136" s="19" t="n"/>
+      <c r="AG136" s="2" t="n"/>
       <c r="AH136" s="2" t="n"/>
       <c r="AI136" s="2" t="n"/>
       <c r="AJ136" s="2" t="n"/>
@@ -15983,18 +15974,18 @@
         </is>
       </c>
       <c r="AC137" s="2" t="n"/>
-      <c r="AD137" s="19" t="inlineStr">
+      <c r="AD137" s="17" t="inlineStr">
         <is>
           <t>18:30</t>
         </is>
       </c>
-      <c r="AE137" s="19" t="n"/>
-      <c r="AF137" s="19" t="inlineStr">
+      <c r="AE137" s="2" t="n"/>
+      <c r="AF137" s="17" t="inlineStr">
         <is>
           <t>18:45</t>
         </is>
       </c>
-      <c r="AG137" s="19" t="n"/>
+      <c r="AG137" s="2" t="n"/>
       <c r="AH137" s="2" t="n"/>
       <c r="AI137" s="2" t="n"/>
       <c r="AJ137" s="2" t="n"/>
@@ -16862,12 +16853,12 @@
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
       </c>
-      <c r="AD144" s="19" t="inlineStr">
+      <c r="AD144" s="17" t="inlineStr">
         <is>
           <t>08:29</t>
         </is>
       </c>
-      <c r="AE144" s="19" t="inlineStr">
+      <c r="AE144" s="2" t="inlineStr">
         <is>
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
@@ -17006,12 +16997,12 @@
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
       </c>
-      <c r="AD145" s="19" t="inlineStr">
+      <c r="AD145" s="17" t="inlineStr">
         <is>
           <t>17:34</t>
         </is>
       </c>
-      <c r="AE145" s="19" t="inlineStr">
+      <c r="AE145" s="2" t="inlineStr">
         <is>
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
@@ -17157,22 +17148,22 @@
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
       </c>
-      <c r="AD146" s="19" t="inlineStr">
+      <c r="AD146" s="17" t="inlineStr">
         <is>
           <t>08:04</t>
         </is>
       </c>
-      <c r="AE146" s="19" t="inlineStr">
+      <c r="AE146" s="2" t="inlineStr">
         <is>
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
       </c>
-      <c r="AF146" s="19" t="inlineStr">
+      <c r="AF146" s="17" t="inlineStr">
         <is>
           <t>08:08</t>
         </is>
       </c>
-      <c r="AG146" s="19" t="n"/>
+      <c r="AG146" s="2" t="n"/>
       <c r="AH146" s="2" t="n"/>
       <c r="AI146" s="2" t="n"/>
       <c r="AJ146" s="2" t="n"/>
@@ -17305,22 +17296,22 @@
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
       </c>
-      <c r="AD147" s="19" t="inlineStr">
+      <c r="AD147" s="17" t="inlineStr">
         <is>
           <t>17:34</t>
         </is>
       </c>
-      <c r="AE147" s="19" t="inlineStr">
+      <c r="AE147" s="2" t="inlineStr">
         <is>
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
       </c>
-      <c r="AF147" s="19" t="inlineStr">
+      <c r="AF147" s="17" t="inlineStr">
         <is>
           <t>17:31</t>
         </is>
       </c>
-      <c r="AG147" s="19" t="inlineStr">
+      <c r="AG147" s="2" t="inlineStr">
         <is>
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
@@ -17440,18 +17431,18 @@
         </is>
       </c>
       <c r="AC148" s="2" t="n"/>
-      <c r="AD148" s="19" t="inlineStr">
+      <c r="AD148" s="17" t="inlineStr">
         <is>
           <t>09:37</t>
         </is>
       </c>
-      <c r="AE148" s="19" t="n"/>
-      <c r="AF148" s="19" t="inlineStr">
+      <c r="AE148" s="2" t="n"/>
+      <c r="AF148" s="17" t="inlineStr">
         <is>
           <t>09:24</t>
         </is>
       </c>
-      <c r="AG148" s="19" t="n"/>
+      <c r="AG148" s="2" t="n"/>
       <c r="AH148" s="2" t="n"/>
       <c r="AI148" s="2" t="n"/>
       <c r="AJ148" s="2" t="n"/>
@@ -17556,18 +17547,18 @@
         </is>
       </c>
       <c r="AC149" s="2" t="n"/>
-      <c r="AD149" s="19" t="inlineStr">
+      <c r="AD149" s="17" t="inlineStr">
         <is>
           <t>17:08</t>
         </is>
       </c>
-      <c r="AE149" s="19" t="n"/>
-      <c r="AF149" s="19" t="inlineStr">
+      <c r="AE149" s="2" t="n"/>
+      <c r="AF149" s="17" t="inlineStr">
         <is>
           <t>17:12</t>
         </is>
       </c>
-      <c r="AG149" s="19" t="n"/>
+      <c r="AG149" s="2" t="n"/>
       <c r="AH149" s="2" t="n"/>
       <c r="AI149" s="2" t="n"/>
       <c r="AJ149" s="2" t="n"/>
@@ -18147,18 +18138,18 @@
         </is>
       </c>
       <c r="AC154" s="2" t="n"/>
-      <c r="AD154" s="19" t="inlineStr">
+      <c r="AD154" s="17" t="inlineStr">
         <is>
           <t>08:48</t>
         </is>
       </c>
-      <c r="AE154" s="19" t="n"/>
-      <c r="AF154" s="19" t="inlineStr">
+      <c r="AE154" s="2" t="n"/>
+      <c r="AF154" s="17" t="inlineStr">
         <is>
           <t>10:17</t>
         </is>
       </c>
-      <c r="AG154" s="19" t="n"/>
+      <c r="AG154" s="2" t="n"/>
       <c r="AH154" s="2" t="n"/>
       <c r="AI154" s="2" t="n"/>
       <c r="AJ154" s="2" t="n"/>
@@ -18263,18 +18254,18 @@
         </is>
       </c>
       <c r="AC155" s="2" t="n"/>
-      <c r="AD155" s="19" t="inlineStr">
+      <c r="AD155" s="17" t="inlineStr">
         <is>
           <t>18:06</t>
         </is>
       </c>
-      <c r="AE155" s="19" t="n"/>
-      <c r="AF155" s="19" t="inlineStr">
+      <c r="AE155" s="2" t="n"/>
+      <c r="AF155" s="17" t="inlineStr">
         <is>
           <t>18:00</t>
         </is>
       </c>
-      <c r="AG155" s="19" t="n"/>
+      <c r="AG155" s="2" t="n"/>
       <c r="AH155" s="2" t="n"/>
       <c r="AI155" s="2" t="n"/>
       <c r="AJ155" s="2" t="n"/>
@@ -18630,18 +18621,18 @@
         </is>
       </c>
       <c r="AC158" s="2" t="n"/>
-      <c r="AD158" s="19" t="inlineStr">
+      <c r="AD158" s="17" t="inlineStr">
         <is>
           <t>08:29</t>
         </is>
       </c>
-      <c r="AE158" s="19" t="n"/>
-      <c r="AF158" s="19" t="inlineStr">
+      <c r="AE158" s="2" t="n"/>
+      <c r="AF158" s="17" t="inlineStr">
         <is>
           <t>08:42</t>
         </is>
       </c>
-      <c r="AG158" s="19" t="n"/>
+      <c r="AG158" s="2" t="n"/>
       <c r="AH158" s="2" t="n"/>
       <c r="AI158" s="2" t="n"/>
       <c r="AJ158" s="2" t="n"/>
@@ -18746,18 +18737,18 @@
         </is>
       </c>
       <c r="AC159" s="2" t="n"/>
-      <c r="AD159" s="19" t="inlineStr">
+      <c r="AD159" s="17" t="inlineStr">
         <is>
           <t>17:36</t>
         </is>
       </c>
-      <c r="AE159" s="19" t="n"/>
-      <c r="AF159" s="19" t="inlineStr">
+      <c r="AE159" s="2" t="n"/>
+      <c r="AF159" s="17" t="inlineStr">
         <is>
           <t>18:38</t>
         </is>
       </c>
-      <c r="AG159" s="19" t="n"/>
+      <c r="AG159" s="2" t="n"/>
       <c r="AH159" s="2" t="n"/>
       <c r="AI159" s="2" t="n"/>
       <c r="AJ159" s="2" t="n"/>
@@ -19093,18 +19084,18 @@
       <c r="AA162" s="2" t="n"/>
       <c r="AB162" s="2" t="n"/>
       <c r="AC162" s="2" t="n"/>
-      <c r="AD162" s="19" t="inlineStr">
+      <c r="AD162" s="17" t="inlineStr">
         <is>
           <t>09:01</t>
         </is>
       </c>
-      <c r="AE162" s="19" t="n"/>
-      <c r="AF162" s="19" t="inlineStr">
+      <c r="AE162" s="2" t="n"/>
+      <c r="AF162" s="17" t="inlineStr">
         <is>
           <t>08:42</t>
         </is>
       </c>
-      <c r="AG162" s="19" t="n"/>
+      <c r="AG162" s="2" t="n"/>
       <c r="AH162" s="2" t="n"/>
       <c r="AI162" s="2" t="n"/>
       <c r="AJ162" s="2" t="n"/>
@@ -19189,18 +19180,18 @@
       <c r="AA163" s="2" t="n"/>
       <c r="AB163" s="2" t="n"/>
       <c r="AC163" s="2" t="n"/>
-      <c r="AD163" s="19" t="inlineStr">
+      <c r="AD163" s="17" t="inlineStr">
         <is>
           <t>18:41</t>
         </is>
       </c>
-      <c r="AE163" s="19" t="n"/>
-      <c r="AF163" s="19" t="inlineStr">
+      <c r="AE163" s="2" t="n"/>
+      <c r="AF163" s="17" t="inlineStr">
         <is>
           <t>18:53</t>
         </is>
       </c>
-      <c r="AG163" s="19" t="n"/>
+      <c r="AG163" s="2" t="n"/>
       <c r="AH163" s="2" t="n"/>
       <c r="AI163" s="2" t="n"/>
       <c r="AJ163" s="2" t="n"/>
@@ -19318,12 +19309,12 @@
         </is>
       </c>
       <c r="AE164" s="2" t="n"/>
-      <c r="AF164" s="19" t="inlineStr">
+      <c r="AF164" s="17" t="inlineStr">
         <is>
           <t>07:50</t>
         </is>
       </c>
-      <c r="AG164" s="19" t="n"/>
+      <c r="AG164" s="2" t="n"/>
       <c r="AH164" s="2" t="n"/>
       <c r="AI164" s="2" t="n"/>
       <c r="AJ164" s="2" t="n"/>
@@ -19430,12 +19421,12 @@
         </is>
       </c>
       <c r="AE165" s="2" t="n"/>
-      <c r="AF165" s="19" t="inlineStr">
+      <c r="AF165" s="17" t="inlineStr">
         <is>
           <t>17:48</t>
         </is>
       </c>
-      <c r="AG165" s="19" t="n"/>
+      <c r="AG165" s="2" t="n"/>
       <c r="AH165" s="2" t="n"/>
       <c r="AI165" s="2" t="n"/>
       <c r="AJ165" s="2" t="n"/>
@@ -19547,12 +19538,12 @@
         </is>
       </c>
       <c r="AC166" s="2" t="n"/>
-      <c r="AD166" s="19" t="inlineStr">
+      <c r="AD166" s="17" t="inlineStr">
         <is>
           <t>07:42</t>
         </is>
       </c>
-      <c r="AE166" s="19" t="n"/>
+      <c r="AE166" s="2" t="n"/>
       <c r="AF166" s="2" t="inlineStr">
         <is>
           <t>07:45</t>
@@ -19659,12 +19650,12 @@
         </is>
       </c>
       <c r="AC167" s="2" t="n"/>
-      <c r="AD167" s="19" t="inlineStr">
+      <c r="AD167" s="17" t="inlineStr">
         <is>
           <t>17:33</t>
         </is>
       </c>
-      <c r="AE167" s="19" t="n"/>
+      <c r="AE167" s="2" t="n"/>
       <c r="AF167" s="2" t="inlineStr">
         <is>
           <t>13:18</t>
@@ -19780,12 +19771,12 @@
       <c r="AC168" s="2" t="n"/>
       <c r="AD168" s="2" t="n"/>
       <c r="AE168" s="2" t="n"/>
-      <c r="AF168" s="19" t="inlineStr">
+      <c r="AF168" s="17" t="inlineStr">
         <is>
           <t>07:32</t>
         </is>
       </c>
-      <c r="AG168" s="19" t="n"/>
+      <c r="AG168" s="2" t="n"/>
       <c r="AH168" s="2" t="n"/>
       <c r="AI168" s="2" t="n"/>
       <c r="AJ168" s="2" t="n"/>
@@ -19884,12 +19875,12 @@
       <c r="AC169" s="2" t="n"/>
       <c r="AD169" s="2" t="n"/>
       <c r="AE169" s="2" t="n"/>
-      <c r="AF169" s="19" t="inlineStr">
+      <c r="AF169" s="17" t="inlineStr">
         <is>
           <t>18:44</t>
         </is>
       </c>
-      <c r="AG169" s="19" t="n"/>
+      <c r="AG169" s="2" t="n"/>
       <c r="AH169" s="2" t="n"/>
       <c r="AI169" s="2" t="n"/>
       <c r="AJ169" s="2" t="n"/>
@@ -20023,12 +20014,12 @@
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
       </c>
-      <c r="AF170" s="19" t="inlineStr">
+      <c r="AF170" s="17" t="inlineStr">
         <is>
           <t>08:45</t>
         </is>
       </c>
-      <c r="AG170" s="19" t="n"/>
+      <c r="AG170" s="2" t="n"/>
       <c r="AH170" s="2" t="n"/>
       <c r="AI170" s="2" t="n"/>
       <c r="AJ170" s="2" t="n"/>
@@ -20155,12 +20146,12 @@
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
       </c>
-      <c r="AF171" s="19" t="inlineStr">
+      <c r="AF171" s="17" t="inlineStr">
         <is>
           <t>17:31</t>
         </is>
       </c>
-      <c r="AG171" s="19" t="inlineStr">
+      <c r="AG171" s="2" t="inlineStr">
         <is>
           <t>Return Home Bus 2024(Return Home Bus 2024)</t>
         </is>
@@ -20264,18 +20255,18 @@
       <c r="AA172" s="2" t="n"/>
       <c r="AB172" s="2" t="n"/>
       <c r="AC172" s="2" t="n"/>
-      <c r="AD172" s="19" t="inlineStr">
+      <c r="AD172" s="17" t="inlineStr">
         <is>
           <t>08:31</t>
         </is>
       </c>
-      <c r="AE172" s="19" t="n"/>
-      <c r="AF172" s="19" t="inlineStr">
+      <c r="AE172" s="2" t="n"/>
+      <c r="AF172" s="17" t="inlineStr">
         <is>
           <t>08:25</t>
         </is>
       </c>
-      <c r="AG172" s="19" t="n"/>
+      <c r="AG172" s="2" t="n"/>
       <c r="AH172" s="2" t="n"/>
       <c r="AI172" s="2" t="n"/>
       <c r="AJ172" s="2" t="n"/>
@@ -20364,18 +20355,18 @@
       <c r="AA173" s="2" t="n"/>
       <c r="AB173" s="2" t="n"/>
       <c r="AC173" s="2" t="n"/>
-      <c r="AD173" s="19" t="inlineStr">
+      <c r="AD173" s="17" t="inlineStr">
         <is>
           <t>17:32</t>
         </is>
       </c>
-      <c r="AE173" s="19" t="n"/>
-      <c r="AF173" s="19" t="inlineStr">
+      <c r="AE173" s="2" t="n"/>
+      <c r="AF173" s="17" t="inlineStr">
         <is>
           <t>17:49</t>
         </is>
       </c>
-      <c r="AG173" s="19" t="n"/>
+      <c r="AG173" s="2" t="n"/>
       <c r="AH173" s="2" t="n"/>
       <c r="AI173" s="2" t="n"/>
       <c r="AJ173" s="2" t="n"/>
@@ -20487,18 +20478,18 @@
         </is>
       </c>
       <c r="AC174" s="2" t="n"/>
-      <c r="AD174" s="19" t="inlineStr">
+      <c r="AD174" s="17" t="inlineStr">
         <is>
           <t>08:40</t>
         </is>
       </c>
-      <c r="AE174" s="19" t="n"/>
-      <c r="AF174" s="19" t="inlineStr">
+      <c r="AE174" s="2" t="n"/>
+      <c r="AF174" s="17" t="inlineStr">
         <is>
           <t>08:32</t>
         </is>
       </c>
-      <c r="AG174" s="19" t="n"/>
+      <c r="AG174" s="2" t="n"/>
       <c r="AH174" s="2" t="n"/>
       <c r="AI174" s="2" t="n"/>
       <c r="AJ174" s="2" t="n"/>
@@ -20599,18 +20590,18 @@
         </is>
       </c>
       <c r="AC175" s="2" t="n"/>
-      <c r="AD175" s="19" t="inlineStr">
+      <c r="AD175" s="17" t="inlineStr">
         <is>
           <t>18:06</t>
         </is>
       </c>
-      <c r="AE175" s="19" t="n"/>
-      <c r="AF175" s="19" t="inlineStr">
+      <c r="AE175" s="2" t="n"/>
+      <c r="AF175" s="17" t="inlineStr">
         <is>
           <t>17:55</t>
         </is>
       </c>
-      <c r="AG175" s="19" t="n"/>
+      <c r="AG175" s="2" t="n"/>
       <c r="AH175" s="2" t="n"/>
       <c r="AI175" s="2" t="n"/>
       <c r="AJ175" s="2" t="n"/>
@@ -21142,18 +21133,18 @@
       <c r="AA180" s="2" t="n"/>
       <c r="AB180" s="2" t="n"/>
       <c r="AC180" s="2" t="n"/>
-      <c r="AD180" s="19" t="inlineStr">
+      <c r="AD180" s="17" t="inlineStr">
         <is>
           <t>08:06</t>
         </is>
       </c>
-      <c r="AE180" s="19" t="n"/>
-      <c r="AF180" s="19" t="inlineStr">
+      <c r="AE180" s="2" t="n"/>
+      <c r="AF180" s="17" t="inlineStr">
         <is>
           <t>08:17</t>
         </is>
       </c>
-      <c r="AG180" s="19" t="n"/>
+      <c r="AG180" s="2" t="n"/>
       <c r="AH180" s="2" t="n"/>
       <c r="AI180" s="2" t="n"/>
       <c r="AJ180" s="2" t="n"/>
@@ -21250,18 +21241,18 @@
       <c r="AA181" s="2" t="n"/>
       <c r="AB181" s="2" t="n"/>
       <c r="AC181" s="2" t="n"/>
-      <c r="AD181" s="19" t="inlineStr">
+      <c r="AD181" s="17" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
-      <c r="AE181" s="19" t="n"/>
-      <c r="AF181" s="19" t="inlineStr">
+      <c r="AE181" s="2" t="n"/>
+      <c r="AF181" s="17" t="inlineStr">
         <is>
           <t>16:33</t>
         </is>
       </c>
-      <c r="AG181" s="19" t="n"/>
+      <c r="AG181" s="2" t="n"/>
       <c r="AH181" s="2" t="n"/>
       <c r="AI181" s="2" t="n"/>
       <c r="AJ181" s="2" t="n"/>
@@ -21775,12 +21766,12 @@
       <c r="AC186" s="2" t="n"/>
       <c r="AD186" s="2" t="n"/>
       <c r="AE186" s="2" t="n"/>
-      <c r="AF186" s="19" t="inlineStr">
+      <c r="AF186" s="17" t="inlineStr">
         <is>
           <t>09:04</t>
         </is>
       </c>
-      <c r="AG186" s="19" t="n"/>
+      <c r="AG186" s="2" t="n"/>
       <c r="AH186" s="2" t="n"/>
       <c r="AI186" s="2" t="n"/>
       <c r="AJ186" s="2" t="n"/>
@@ -21875,12 +21866,12 @@
       <c r="AC187" s="2" t="n"/>
       <c r="AD187" s="2" t="n"/>
       <c r="AE187" s="2" t="n"/>
-      <c r="AF187" s="19" t="inlineStr">
+      <c r="AF187" s="17" t="inlineStr">
         <is>
           <t>17:29</t>
         </is>
       </c>
-      <c r="AG187" s="19" t="n"/>
+      <c r="AG187" s="2" t="n"/>
       <c r="AH187" s="2" t="n"/>
       <c r="AI187" s="2" t="n"/>
       <c r="AJ187" s="2" t="n"/>
@@ -21984,18 +21975,18 @@
         </is>
       </c>
       <c r="AC188" s="2" t="n"/>
-      <c r="AD188" s="19" t="inlineStr">
+      <c r="AD188" s="17" t="inlineStr">
         <is>
           <t>08:00</t>
         </is>
       </c>
-      <c r="AE188" s="19" t="n"/>
-      <c r="AF188" s="19" t="inlineStr">
+      <c r="AE188" s="2" t="n"/>
+      <c r="AF188" s="17" t="inlineStr">
         <is>
           <t>08:08</t>
         </is>
       </c>
-      <c r="AG188" s="19" t="n"/>
+      <c r="AG188" s="2" t="n"/>
       <c r="AH188" s="2" t="n"/>
       <c r="AI188" s="2" t="n"/>
       <c r="AJ188" s="2" t="n"/>
@@ -22088,18 +22079,18 @@
         </is>
       </c>
       <c r="AC189" s="2" t="n"/>
-      <c r="AD189" s="19" t="inlineStr">
+      <c r="AD189" s="17" t="inlineStr">
         <is>
           <t>17:47</t>
         </is>
       </c>
-      <c r="AE189" s="19" t="n"/>
-      <c r="AF189" s="19" t="inlineStr">
+      <c r="AE189" s="2" t="n"/>
+      <c r="AF189" s="17" t="inlineStr">
         <is>
           <t>18:06</t>
         </is>
       </c>
-      <c r="AG189" s="19" t="n"/>
+      <c r="AG189" s="2" t="n"/>
       <c r="AH189" s="2" t="n"/>
       <c r="AI189" s="2" t="n"/>
       <c r="AJ189" s="2" t="n"/>
@@ -22451,18 +22442,18 @@
         </is>
       </c>
       <c r="AC192" s="2" t="n"/>
-      <c r="AD192" s="19" t="inlineStr">
+      <c r="AD192" s="17" t="inlineStr">
         <is>
           <t>08:12</t>
         </is>
       </c>
-      <c r="AE192" s="19" t="n"/>
-      <c r="AF192" s="19" t="inlineStr">
+      <c r="AE192" s="2" t="n"/>
+      <c r="AF192" s="17" t="inlineStr">
         <is>
           <t>08:10</t>
         </is>
       </c>
-      <c r="AG192" s="19" t="n"/>
+      <c r="AG192" s="2" t="n"/>
       <c r="AH192" s="2" t="n"/>
       <c r="AI192" s="2" t="n"/>
       <c r="AJ192" s="2" t="n"/>
@@ -22563,18 +22554,18 @@
         </is>
       </c>
       <c r="AC193" s="2" t="n"/>
-      <c r="AD193" s="19" t="inlineStr">
+      <c r="AD193" s="17" t="inlineStr">
         <is>
           <t>18:21</t>
         </is>
       </c>
-      <c r="AE193" s="19" t="n"/>
-      <c r="AF193" s="19" t="inlineStr">
+      <c r="AE193" s="2" t="n"/>
+      <c r="AF193" s="17" t="inlineStr">
         <is>
           <t>18:23</t>
         </is>
       </c>
-      <c r="AG193" s="19" t="n"/>
+      <c r="AG193" s="2" t="n"/>
       <c r="AH193" s="2" t="n"/>
       <c r="AI193" s="2" t="n"/>
       <c r="AJ193" s="2" t="n"/>
@@ -23142,12 +23133,12 @@
         </is>
       </c>
       <c r="AC198" s="2" t="n"/>
-      <c r="AD198" s="19" t="inlineStr">
+      <c r="AD198" s="17" t="inlineStr">
         <is>
           <t>08:13</t>
         </is>
       </c>
-      <c r="AE198" s="19" t="n"/>
+      <c r="AE198" s="2" t="n"/>
       <c r="AF198" s="2" t="n"/>
       <c r="AG198" s="2" t="n"/>
       <c r="AH198" s="2" t="n"/>
@@ -23250,12 +23241,12 @@
         </is>
       </c>
       <c r="AC199" s="2" t="n"/>
-      <c r="AD199" s="19" t="inlineStr">
+      <c r="AD199" s="17" t="inlineStr">
         <is>
           <t>18:06</t>
         </is>
       </c>
-      <c r="AE199" s="19" t="n"/>
+      <c r="AE199" s="2" t="n"/>
       <c r="AF199" s="2" t="n"/>
       <c r="AG199" s="2" t="n"/>
       <c r="AH199" s="2" t="n"/>

</xml_diff>